<commit_message>
Refactor logging system configuration
</commit_message>
<xml_diff>
--- a/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
+++ b/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I472"/>
+  <dimension ref="A1:I475"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17842,7 +17842,7 @@
     </row>
     <row r="471">
       <c r="A471" s="2" t="n">
-        <v>45725.23113506944</v>
+        <v>45725.23111297454</v>
       </c>
       <c r="B471" t="inlineStr">
         <is>
@@ -17879,38 +17879,149 @@
     </row>
     <row r="472">
       <c r="A472" s="2" t="n">
+        <v>45725.23113506944</v>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F472" t="n">
+        <v>400</v>
+      </c>
+      <c r="G472" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H472" t="n">
+        <v>400</v>
+      </c>
+      <c r="I472" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="2" t="n">
+        <v>45725.23113506944</v>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F473" t="n">
+        <v>400</v>
+      </c>
+      <c r="G473" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H473" t="n">
+        <v>400</v>
+      </c>
+      <c r="I473" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="2" t="n">
         <v>45725.23115855324</v>
       </c>
-      <c r="B472" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C472" t="inlineStr">
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D472" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E472" t="inlineStr">
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E474" t="inlineStr">
         <is>
           <t>0xd</t>
         </is>
       </c>
-      <c r="F472" t="n">
-        <v>400</v>
-      </c>
-      <c r="G472" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H472" t="n">
-        <v>400</v>
-      </c>
-      <c r="I472" t="n">
+      <c r="F474" t="n">
+        <v>400</v>
+      </c>
+      <c r="G474" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H474" t="n">
+        <v>400</v>
+      </c>
+      <c r="I474" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="2" t="n">
+        <v>45725.23115855324</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F475" t="n">
+        <v>400</v>
+      </c>
+      <c r="G475" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H475" t="n">
+        <v>400</v>
+      </c>
+      <c r="I475" t="n">
         <v>13</v>
       </c>
     </row>
@@ -17925,7 +18036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I486"/>
+  <dimension ref="A1:I489"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35853,7 +35964,7 @@
     </row>
     <row r="485">
       <c r="A485" s="2" t="n">
-        <v>45725.07911518519</v>
+        <v>45725.07909302083</v>
       </c>
       <c r="B485" t="inlineStr">
         <is>
@@ -35890,38 +36001,149 @@
     </row>
     <row r="486">
       <c r="A486" s="2" t="n">
+        <v>45725.07911518519</v>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F486" t="n">
+        <v>400</v>
+      </c>
+      <c r="G486" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H486" t="n">
+        <v>400</v>
+      </c>
+      <c r="I486" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="2" t="n">
+        <v>45725.07911518519</v>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F487" t="n">
+        <v>400</v>
+      </c>
+      <c r="G487" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H487" t="n">
+        <v>400</v>
+      </c>
+      <c r="I487" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="2" t="n">
         <v>45725.07913833333</v>
       </c>
-      <c r="B486" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C486" t="inlineStr">
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D486" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E486" t="inlineStr">
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
         <is>
           <t>0xe</t>
         </is>
       </c>
-      <c r="F486" t="n">
-        <v>400</v>
-      </c>
-      <c r="G486" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H486" t="n">
-        <v>400</v>
-      </c>
-      <c r="I486" t="n">
+      <c r="F488" t="n">
+        <v>400</v>
+      </c>
+      <c r="G488" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H488" t="n">
+        <v>400</v>
+      </c>
+      <c r="I488" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="2" t="n">
+        <v>45725.07913833333</v>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F489" t="n">
+        <v>400</v>
+      </c>
+      <c r="G489" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H489" t="n">
+        <v>400</v>
+      </c>
+      <c r="I489" t="n">
         <v>14</v>
       </c>
     </row>
@@ -51986,7 +52208,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I490"/>
+  <dimension ref="A1:I493"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -70062,7 +70284,7 @@
     </row>
     <row r="489">
       <c r="A489" s="2" t="n">
-        <v>45725.22922125</v>
+        <v>45725.22919952546</v>
       </c>
       <c r="B489" t="inlineStr">
         <is>
@@ -70099,38 +70321,149 @@
     </row>
     <row r="490">
       <c r="A490" s="2" t="n">
+        <v>45725.22922125</v>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F490" t="n">
+        <v>400</v>
+      </c>
+      <c r="G490" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H490" t="n">
+        <v>400</v>
+      </c>
+      <c r="I490" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="2" t="n">
+        <v>45725.22922125</v>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F491" t="n">
+        <v>400</v>
+      </c>
+      <c r="G491" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H491" t="n">
+        <v>400</v>
+      </c>
+      <c r="I491" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="2" t="n">
         <v>45725.22924497685</v>
       </c>
-      <c r="B490" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C490" t="inlineStr">
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
         </is>
       </c>
-      <c r="D490" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E490" t="inlineStr">
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
         <is>
           <t>0x3</t>
         </is>
       </c>
-      <c r="F490" t="n">
-        <v>400</v>
-      </c>
-      <c r="G490" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H490" t="n">
-        <v>400</v>
-      </c>
-      <c r="I490" t="n">
+      <c r="F492" t="n">
+        <v>400</v>
+      </c>
+      <c r="G492" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H492" t="n">
+        <v>400</v>
+      </c>
+      <c r="I492" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="2" t="n">
+        <v>45725.22924497685</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F493" t="n">
+        <v>400</v>
+      </c>
+      <c r="G493" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H493" t="n">
+        <v>400</v>
+      </c>
+      <c r="I493" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Optimize error message display
</commit_message>
<xml_diff>
--- a/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
+++ b/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I475"/>
+  <dimension ref="A1:I481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17879,7 +17879,7 @@
     </row>
     <row r="472">
       <c r="A472" s="2" t="n">
-        <v>45725.23113506944</v>
+        <v>45725.23111297454</v>
       </c>
       <c r="B472" t="inlineStr">
         <is>
@@ -17953,7 +17953,7 @@
     </row>
     <row r="474">
       <c r="A474" s="2" t="n">
-        <v>45725.23115855324</v>
+        <v>45725.23113506944</v>
       </c>
       <c r="B474" t="inlineStr">
         <is>
@@ -17990,38 +17990,260 @@
     </row>
     <row r="475">
       <c r="A475" s="2" t="n">
+        <v>45725.23113506944</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F475" t="n">
+        <v>400</v>
+      </c>
+      <c r="G475" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H475" t="n">
+        <v>400</v>
+      </c>
+      <c r="I475" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="2" t="n">
         <v>45725.23115855324</v>
       </c>
-      <c r="B475" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C475" t="inlineStr">
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D475" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E475" t="inlineStr">
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E476" t="inlineStr">
         <is>
           <t>0xd</t>
         </is>
       </c>
-      <c r="F475" t="n">
-        <v>400</v>
-      </c>
-      <c r="G475" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H475" t="n">
-        <v>400</v>
-      </c>
-      <c r="I475" t="n">
+      <c r="F476" t="n">
+        <v>400</v>
+      </c>
+      <c r="G476" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H476" t="n">
+        <v>400</v>
+      </c>
+      <c r="I476" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="2" t="n">
+        <v>45725.23115855324</v>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F477" t="n">
+        <v>400</v>
+      </c>
+      <c r="G477" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H477" t="n">
+        <v>400</v>
+      </c>
+      <c r="I477" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="2" t="n">
+        <v>45725.23115855324</v>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F478" t="n">
+        <v>400</v>
+      </c>
+      <c r="G478" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H478" t="n">
+        <v>400</v>
+      </c>
+      <c r="I478" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="2" t="n">
+        <v>45725.73125641204</v>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F479" t="n">
+        <v>400</v>
+      </c>
+      <c r="G479" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H479" t="n">
+        <v>400</v>
+      </c>
+      <c r="I479" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="2" t="n">
+        <v>45725.73127832176</v>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F480" t="n">
+        <v>400</v>
+      </c>
+      <c r="G480" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H480" t="n">
+        <v>400</v>
+      </c>
+      <c r="I480" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="2" t="n">
+        <v>45725.73130123843</v>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F481" t="n">
+        <v>400</v>
+      </c>
+      <c r="G481" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H481" t="n">
+        <v>400</v>
+      </c>
+      <c r="I481" t="n">
         <v>13</v>
       </c>
     </row>
@@ -18036,7 +18258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I489"/>
+  <dimension ref="A1:I495"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36001,7 +36223,7 @@
     </row>
     <row r="486">
       <c r="A486" s="2" t="n">
-        <v>45725.07911518519</v>
+        <v>45725.07909302083</v>
       </c>
       <c r="B486" t="inlineStr">
         <is>
@@ -36075,7 +36297,7 @@
     </row>
     <row r="488">
       <c r="A488" s="2" t="n">
-        <v>45725.07913833333</v>
+        <v>45725.07911518519</v>
       </c>
       <c r="B488" t="inlineStr">
         <is>
@@ -36112,38 +36334,260 @@
     </row>
     <row r="489">
       <c r="A489" s="2" t="n">
+        <v>45725.07911518519</v>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F489" t="n">
+        <v>400</v>
+      </c>
+      <c r="G489" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H489" t="n">
+        <v>400</v>
+      </c>
+      <c r="I489" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="2" t="n">
         <v>45725.07913833333</v>
       </c>
-      <c r="B489" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C489" t="inlineStr">
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D489" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E489" t="inlineStr">
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
         <is>
           <t>0xe</t>
         </is>
       </c>
-      <c r="F489" t="n">
-        <v>400</v>
-      </c>
-      <c r="G489" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H489" t="n">
-        <v>400</v>
-      </c>
-      <c r="I489" t="n">
+      <c r="F490" t="n">
+        <v>400</v>
+      </c>
+      <c r="G490" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H490" t="n">
+        <v>400</v>
+      </c>
+      <c r="I490" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="2" t="n">
+        <v>45725.07913833333</v>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F491" t="n">
+        <v>400</v>
+      </c>
+      <c r="G491" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H491" t="n">
+        <v>400</v>
+      </c>
+      <c r="I491" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="2" t="n">
+        <v>45725.07913833333</v>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F492" t="n">
+        <v>400</v>
+      </c>
+      <c r="G492" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H492" t="n">
+        <v>400</v>
+      </c>
+      <c r="I492" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="2" t="n">
+        <v>45725.57923533564</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F493" t="n">
+        <v>400</v>
+      </c>
+      <c r="G493" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H493" t="n">
+        <v>400</v>
+      </c>
+      <c r="I493" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="2" t="n">
+        <v>45725.57925716435</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F494" t="n">
+        <v>400</v>
+      </c>
+      <c r="G494" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H494" t="n">
+        <v>400</v>
+      </c>
+      <c r="I494" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="2" t="n">
+        <v>45725.57928042824</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F495" t="n">
+        <v>400</v>
+      </c>
+      <c r="G495" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H495" t="n">
+        <v>400</v>
+      </c>
+      <c r="I495" t="n">
         <v>14</v>
       </c>
     </row>
@@ -52208,7 +52652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I493"/>
+  <dimension ref="A1:I499"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -70321,7 +70765,7 @@
     </row>
     <row r="490">
       <c r="A490" s="2" t="n">
-        <v>45725.22922125</v>
+        <v>45725.22919952546</v>
       </c>
       <c r="B490" t="inlineStr">
         <is>
@@ -70395,7 +70839,7 @@
     </row>
     <row r="492">
       <c r="A492" s="2" t="n">
-        <v>45725.22924497685</v>
+        <v>45725.22922125</v>
       </c>
       <c r="B492" t="inlineStr">
         <is>
@@ -70432,38 +70876,260 @@
     </row>
     <row r="493">
       <c r="A493" s="2" t="n">
+        <v>45725.22922125</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F493" t="n">
+        <v>400</v>
+      </c>
+      <c r="G493" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H493" t="n">
+        <v>400</v>
+      </c>
+      <c r="I493" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="2" t="n">
         <v>45725.22924497685</v>
       </c>
-      <c r="B493" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C493" t="inlineStr">
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
         </is>
       </c>
-      <c r="D493" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E493" t="inlineStr">
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
         <is>
           <t>0x3</t>
         </is>
       </c>
-      <c r="F493" t="n">
-        <v>400</v>
-      </c>
-      <c r="G493" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H493" t="n">
-        <v>400</v>
-      </c>
-      <c r="I493" t="n">
+      <c r="F494" t="n">
+        <v>400</v>
+      </c>
+      <c r="G494" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H494" t="n">
+        <v>400</v>
+      </c>
+      <c r="I494" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="2" t="n">
+        <v>45725.22924497685</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F495" t="n">
+        <v>400</v>
+      </c>
+      <c r="G495" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H495" t="n">
+        <v>400</v>
+      </c>
+      <c r="I495" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="2" t="n">
+        <v>45725.22924497685</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F496" t="n">
+        <v>400</v>
+      </c>
+      <c r="G496" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H496" t="n">
+        <v>400</v>
+      </c>
+      <c r="I496" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="2" t="n">
+        <v>45725.7293421412</v>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F497" t="n">
+        <v>400</v>
+      </c>
+      <c r="G497" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H497" t="n">
+        <v>400</v>
+      </c>
+      <c r="I497" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="2" t="n">
+        <v>45725.72936453704</v>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F498" t="n">
+        <v>400</v>
+      </c>
+      <c r="G498" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H498" t="n">
+        <v>400</v>
+      </c>
+      <c r="I498" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="2" t="n">
+        <v>45725.7293875</v>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F499" t="n">
+        <v>400</v>
+      </c>
+      <c r="G499" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H499" t="n">
+        <v>400</v>
+      </c>
+      <c r="I499" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve unit test coverage
</commit_message>
<xml_diff>
--- a/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
+++ b/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I487"/>
+  <dimension ref="A1:I496"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17953,7 +17953,7 @@
     </row>
     <row r="474">
       <c r="A474" s="2" t="n">
-        <v>45725.23113506944</v>
+        <v>45725.23111297454</v>
       </c>
       <c r="B474" t="inlineStr">
         <is>
@@ -18101,7 +18101,7 @@
     </row>
     <row r="478">
       <c r="A478" s="2" t="n">
-        <v>45725.23115855324</v>
+        <v>45725.23113506944</v>
       </c>
       <c r="B478" t="inlineStr">
         <is>
@@ -18138,7 +18138,7 @@
     </row>
     <row r="479">
       <c r="A479" s="2" t="n">
-        <v>45725.23115855324</v>
+        <v>45725.23113506944</v>
       </c>
       <c r="B479" t="inlineStr">
         <is>
@@ -18249,7 +18249,7 @@
     </row>
     <row r="482">
       <c r="A482" s="2" t="n">
-        <v>45725.73125641204</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B482" t="inlineStr">
         <is>
@@ -18286,7 +18286,7 @@
     </row>
     <row r="483">
       <c r="A483" s="2" t="n">
-        <v>45725.73125641204</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B483" t="inlineStr">
         <is>
@@ -18323,7 +18323,7 @@
     </row>
     <row r="484">
       <c r="A484" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B484" t="inlineStr">
         <is>
@@ -18360,7 +18360,7 @@
     </row>
     <row r="485">
       <c r="A485" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B485" t="inlineStr">
         <is>
@@ -18397,7 +18397,7 @@
     </row>
     <row r="486">
       <c r="A486" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B486" t="inlineStr">
         <is>
@@ -18434,38 +18434,371 @@
     </row>
     <row r="487">
       <c r="A487" s="2" t="n">
+        <v>45725.73125641204</v>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F487" t="n">
+        <v>400</v>
+      </c>
+      <c r="G487" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H487" t="n">
+        <v>400</v>
+      </c>
+      <c r="I487" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="2" t="n">
+        <v>45725.73127832176</v>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F488" t="n">
+        <v>400</v>
+      </c>
+      <c r="G488" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H488" t="n">
+        <v>400</v>
+      </c>
+      <c r="I488" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="2" t="n">
+        <v>45725.73127832176</v>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F489" t="n">
+        <v>400</v>
+      </c>
+      <c r="G489" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H489" t="n">
+        <v>400</v>
+      </c>
+      <c r="I489" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="2" t="n">
+        <v>45725.73127832176</v>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F490" t="n">
+        <v>400</v>
+      </c>
+      <c r="G490" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H490" t="n">
+        <v>400</v>
+      </c>
+      <c r="I490" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="2" t="n">
         <v>45725.73130123843</v>
       </c>
-      <c r="B487" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C487" t="inlineStr">
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D487" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E487" t="inlineStr">
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
         <is>
           <t>0xd</t>
         </is>
       </c>
-      <c r="F487" t="n">
-        <v>400</v>
-      </c>
-      <c r="G487" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H487" t="n">
-        <v>400</v>
-      </c>
-      <c r="I487" t="n">
+      <c r="F491" t="n">
+        <v>400</v>
+      </c>
+      <c r="G491" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H491" t="n">
+        <v>400</v>
+      </c>
+      <c r="I491" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="2" t="n">
+        <v>45725.73130123843</v>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F492" t="n">
+        <v>400</v>
+      </c>
+      <c r="G492" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H492" t="n">
+        <v>400</v>
+      </c>
+      <c r="I492" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="2" t="n">
+        <v>45725.73130123843</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F493" t="n">
+        <v>400</v>
+      </c>
+      <c r="G493" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H493" t="n">
+        <v>400</v>
+      </c>
+      <c r="I493" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="2" t="n">
+        <v>45726.23139893518</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F494" t="n">
+        <v>400</v>
+      </c>
+      <c r="G494" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H494" t="n">
+        <v>400</v>
+      </c>
+      <c r="I494" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="2" t="n">
+        <v>45726.23142038195</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F495" t="n">
+        <v>400</v>
+      </c>
+      <c r="G495" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H495" t="n">
+        <v>400</v>
+      </c>
+      <c r="I495" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="2" t="n">
+        <v>45726.23144357639</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F496" t="n">
+        <v>400</v>
+      </c>
+      <c r="G496" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H496" t="n">
+        <v>400</v>
+      </c>
+      <c r="I496" t="n">
         <v>13</v>
       </c>
     </row>
@@ -18480,7 +18813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I501"/>
+  <dimension ref="A1:I510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36519,7 +36852,7 @@
     </row>
     <row r="488">
       <c r="A488" s="2" t="n">
-        <v>45725.07911518519</v>
+        <v>45725.07909302083</v>
       </c>
       <c r="B488" t="inlineStr">
         <is>
@@ -36667,7 +37000,7 @@
     </row>
     <row r="492">
       <c r="A492" s="2" t="n">
-        <v>45725.07913833333</v>
+        <v>45725.07911518519</v>
       </c>
       <c r="B492" t="inlineStr">
         <is>
@@ -36704,7 +37037,7 @@
     </row>
     <row r="493">
       <c r="A493" s="2" t="n">
-        <v>45725.07913833333</v>
+        <v>45725.07911518519</v>
       </c>
       <c r="B493" t="inlineStr">
         <is>
@@ -36815,7 +37148,7 @@
     </row>
     <row r="496">
       <c r="A496" s="2" t="n">
-        <v>45725.57923533564</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B496" t="inlineStr">
         <is>
@@ -36852,7 +37185,7 @@
     </row>
     <row r="497">
       <c r="A497" s="2" t="n">
-        <v>45725.57923533564</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B497" t="inlineStr">
         <is>
@@ -36889,7 +37222,7 @@
     </row>
     <row r="498">
       <c r="A498" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B498" t="inlineStr">
         <is>
@@ -36926,7 +37259,7 @@
     </row>
     <row r="499">
       <c r="A499" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B499" t="inlineStr">
         <is>
@@ -36963,7 +37296,7 @@
     </row>
     <row r="500">
       <c r="A500" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B500" t="inlineStr">
         <is>
@@ -37000,38 +37333,371 @@
     </row>
     <row r="501">
       <c r="A501" s="2" t="n">
+        <v>45725.57923533564</v>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F501" t="n">
+        <v>400</v>
+      </c>
+      <c r="G501" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H501" t="n">
+        <v>400</v>
+      </c>
+      <c r="I501" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="2" t="n">
+        <v>45725.57925716435</v>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F502" t="n">
+        <v>400</v>
+      </c>
+      <c r="G502" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H502" t="n">
+        <v>400</v>
+      </c>
+      <c r="I502" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="2" t="n">
+        <v>45725.57925716435</v>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F503" t="n">
+        <v>400</v>
+      </c>
+      <c r="G503" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H503" t="n">
+        <v>400</v>
+      </c>
+      <c r="I503" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="2" t="n">
+        <v>45725.57925716435</v>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F504" t="n">
+        <v>400</v>
+      </c>
+      <c r="G504" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H504" t="n">
+        <v>400</v>
+      </c>
+      <c r="I504" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="2" t="n">
         <v>45725.57928042824</v>
       </c>
-      <c r="B501" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C501" t="inlineStr">
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D501" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E501" t="inlineStr">
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr">
         <is>
           <t>0xe</t>
         </is>
       </c>
-      <c r="F501" t="n">
-        <v>400</v>
-      </c>
-      <c r="G501" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H501" t="n">
-        <v>400</v>
-      </c>
-      <c r="I501" t="n">
+      <c r="F505" t="n">
+        <v>400</v>
+      </c>
+      <c r="G505" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H505" t="n">
+        <v>400</v>
+      </c>
+      <c r="I505" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="2" t="n">
+        <v>45725.57928042824</v>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F506" t="n">
+        <v>400</v>
+      </c>
+      <c r="G506" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H506" t="n">
+        <v>400</v>
+      </c>
+      <c r="I506" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="2" t="n">
+        <v>45725.57928042824</v>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F507" t="n">
+        <v>400</v>
+      </c>
+      <c r="G507" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H507" t="n">
+        <v>400</v>
+      </c>
+      <c r="I507" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="2" t="n">
+        <v>45726.07937777778</v>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E508" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F508" t="n">
+        <v>400</v>
+      </c>
+      <c r="G508" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H508" t="n">
+        <v>400</v>
+      </c>
+      <c r="I508" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="2" t="n">
+        <v>45726.07939922454</v>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F509" t="n">
+        <v>400</v>
+      </c>
+      <c r="G509" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H509" t="n">
+        <v>400</v>
+      </c>
+      <c r="I509" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="2" t="n">
+        <v>45726.07942256945</v>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F510" t="n">
+        <v>400</v>
+      </c>
+      <c r="G510" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H510" t="n">
+        <v>400</v>
+      </c>
+      <c r="I510" t="n">
         <v>14</v>
       </c>
     </row>
@@ -53096,7 +53762,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I505"/>
+  <dimension ref="A1:I514"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -71283,7 +71949,7 @@
     </row>
     <row r="492">
       <c r="A492" s="2" t="n">
-        <v>45725.22922125</v>
+        <v>45725.22919952546</v>
       </c>
       <c r="B492" t="inlineStr">
         <is>
@@ -71431,7 +72097,7 @@
     </row>
     <row r="496">
       <c r="A496" s="2" t="n">
-        <v>45725.22924497685</v>
+        <v>45725.22922125</v>
       </c>
       <c r="B496" t="inlineStr">
         <is>
@@ -71468,7 +72134,7 @@
     </row>
     <row r="497">
       <c r="A497" s="2" t="n">
-        <v>45725.22924497685</v>
+        <v>45725.22922125</v>
       </c>
       <c r="B497" t="inlineStr">
         <is>
@@ -71579,7 +72245,7 @@
     </row>
     <row r="500">
       <c r="A500" s="2" t="n">
-        <v>45725.7293421412</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B500" t="inlineStr">
         <is>
@@ -71616,7 +72282,7 @@
     </row>
     <row r="501">
       <c r="A501" s="2" t="n">
-        <v>45725.7293421412</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B501" t="inlineStr">
         <is>
@@ -71653,7 +72319,7 @@
     </row>
     <row r="502">
       <c r="A502" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B502" t="inlineStr">
         <is>
@@ -71690,7 +72356,7 @@
     </row>
     <row r="503">
       <c r="A503" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B503" t="inlineStr">
         <is>
@@ -71727,7 +72393,7 @@
     </row>
     <row r="504">
       <c r="A504" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B504" t="inlineStr">
         <is>
@@ -71764,38 +72430,371 @@
     </row>
     <row r="505">
       <c r="A505" s="2" t="n">
+        <v>45725.7293421412</v>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F505" t="n">
+        <v>400</v>
+      </c>
+      <c r="G505" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H505" t="n">
+        <v>400</v>
+      </c>
+      <c r="I505" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="2" t="n">
+        <v>45725.72936453704</v>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F506" t="n">
+        <v>400</v>
+      </c>
+      <c r="G506" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H506" t="n">
+        <v>400</v>
+      </c>
+      <c r="I506" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="2" t="n">
+        <v>45725.72936453704</v>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F507" t="n">
+        <v>400</v>
+      </c>
+      <c r="G507" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H507" t="n">
+        <v>400</v>
+      </c>
+      <c r="I507" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="2" t="n">
+        <v>45725.72936453704</v>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E508" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F508" t="n">
+        <v>400</v>
+      </c>
+      <c r="G508" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H508" t="n">
+        <v>400</v>
+      </c>
+      <c r="I508" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="2" t="n">
         <v>45725.7293875</v>
       </c>
-      <c r="B505" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C505" t="inlineStr">
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
         </is>
       </c>
-      <c r="D505" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E505" t="inlineStr">
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr">
         <is>
           <t>0x3</t>
         </is>
       </c>
-      <c r="F505" t="n">
-        <v>400</v>
-      </c>
-      <c r="G505" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H505" t="n">
-        <v>400</v>
-      </c>
-      <c r="I505" t="n">
+      <c r="F509" t="n">
+        <v>400</v>
+      </c>
+      <c r="G509" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H509" t="n">
+        <v>400</v>
+      </c>
+      <c r="I509" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="2" t="n">
+        <v>45725.7293875</v>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F510" t="n">
+        <v>400</v>
+      </c>
+      <c r="G510" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H510" t="n">
+        <v>400</v>
+      </c>
+      <c r="I510" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="2" t="n">
+        <v>45725.7293875</v>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E511" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F511" t="n">
+        <v>400</v>
+      </c>
+      <c r="G511" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H511" t="n">
+        <v>400</v>
+      </c>
+      <c r="I511" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="2" t="n">
+        <v>45726.2294844213</v>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E512" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F512" t="n">
+        <v>400</v>
+      </c>
+      <c r="G512" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H512" t="n">
+        <v>400</v>
+      </c>
+      <c r="I512" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="2" t="n">
+        <v>45726.22950657408</v>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F513" t="n">
+        <v>400</v>
+      </c>
+      <c r="G513" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H513" t="n">
+        <v>400</v>
+      </c>
+      <c r="I513" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="2" t="n">
+        <v>45726.22953034722</v>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E514" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F514" t="n">
+        <v>400</v>
+      </c>
+      <c r="G514" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H514" t="n">
+        <v>400</v>
+      </c>
+      <c r="I514" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix api endpoint validation
Remove deprecated functions and clean up codebase.
</commit_message>
<xml_diff>
--- a/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
+++ b/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I529"/>
+  <dimension ref="A1:I544"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18101,7 +18101,7 @@
     </row>
     <row r="478">
       <c r="A478" s="2" t="n">
-        <v>45725.23113506944</v>
+        <v>45725.23111297454</v>
       </c>
       <c r="B478" t="inlineStr">
         <is>
@@ -18397,7 +18397,7 @@
     </row>
     <row r="486">
       <c r="A486" s="2" t="n">
-        <v>45725.23115855324</v>
+        <v>45725.23113506944</v>
       </c>
       <c r="B486" t="inlineStr">
         <is>
@@ -18434,7 +18434,7 @@
     </row>
     <row r="487">
       <c r="A487" s="2" t="n">
-        <v>45725.23115855324</v>
+        <v>45725.23113506944</v>
       </c>
       <c r="B487" t="inlineStr">
         <is>
@@ -18693,7 +18693,7 @@
     </row>
     <row r="494">
       <c r="A494" s="2" t="n">
-        <v>45725.73125641204</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B494" t="inlineStr">
         <is>
@@ -18730,7 +18730,7 @@
     </row>
     <row r="495">
       <c r="A495" s="2" t="n">
-        <v>45725.73125641204</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B495" t="inlineStr">
         <is>
@@ -18767,7 +18767,7 @@
     </row>
     <row r="496">
       <c r="A496" s="2" t="n">
-        <v>45725.73125641204</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B496" t="inlineStr">
         <is>
@@ -18915,7 +18915,7 @@
     </row>
     <row r="500">
       <c r="A500" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B500" t="inlineStr">
         <is>
@@ -18952,7 +18952,7 @@
     </row>
     <row r="501">
       <c r="A501" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B501" t="inlineStr">
         <is>
@@ -18989,7 +18989,7 @@
     </row>
     <row r="502">
       <c r="A502" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B502" t="inlineStr">
         <is>
@@ -19026,7 +19026,7 @@
     </row>
     <row r="503">
       <c r="A503" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B503" t="inlineStr">
         <is>
@@ -19137,7 +19137,7 @@
     </row>
     <row r="506">
       <c r="A506" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B506" t="inlineStr">
         <is>
@@ -19174,7 +19174,7 @@
     </row>
     <row r="507">
       <c r="A507" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B507" t="inlineStr">
         <is>
@@ -19211,7 +19211,7 @@
     </row>
     <row r="508">
       <c r="A508" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B508" t="inlineStr">
         <is>
@@ -19248,7 +19248,7 @@
     </row>
     <row r="509">
       <c r="A509" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B509" t="inlineStr">
         <is>
@@ -19285,7 +19285,7 @@
     </row>
     <row r="510">
       <c r="A510" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B510" t="inlineStr">
         <is>
@@ -19359,7 +19359,7 @@
     </row>
     <row r="512">
       <c r="A512" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B512" t="inlineStr">
         <is>
@@ -19396,7 +19396,7 @@
     </row>
     <row r="513">
       <c r="A513" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B513" t="inlineStr">
         <is>
@@ -19433,7 +19433,7 @@
     </row>
     <row r="514">
       <c r="A514" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B514" t="inlineStr">
         <is>
@@ -19470,7 +19470,7 @@
     </row>
     <row r="515">
       <c r="A515" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B515" t="inlineStr">
         <is>
@@ -19507,7 +19507,7 @@
     </row>
     <row r="516">
       <c r="A516" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B516" t="inlineStr">
         <is>
@@ -19544,7 +19544,7 @@
     </row>
     <row r="517">
       <c r="A517" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B517" t="inlineStr">
         <is>
@@ -19581,7 +19581,7 @@
     </row>
     <row r="518">
       <c r="A518" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B518" t="inlineStr">
         <is>
@@ -19618,7 +19618,7 @@
     </row>
     <row r="519">
       <c r="A519" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B519" t="inlineStr">
         <is>
@@ -19655,7 +19655,7 @@
     </row>
     <row r="520">
       <c r="A520" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B520" t="inlineStr">
         <is>
@@ -19692,7 +19692,7 @@
     </row>
     <row r="521">
       <c r="A521" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B521" t="inlineStr">
         <is>
@@ -19729,7 +19729,7 @@
     </row>
     <row r="522">
       <c r="A522" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B522" t="inlineStr">
         <is>
@@ -19766,7 +19766,7 @@
     </row>
     <row r="523">
       <c r="A523" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B523" t="inlineStr">
         <is>
@@ -19803,7 +19803,7 @@
     </row>
     <row r="524">
       <c r="A524" s="2" t="n">
-        <v>45726.73154126157</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B524" t="inlineStr">
         <is>
@@ -19840,7 +19840,7 @@
     </row>
     <row r="525">
       <c r="A525" s="2" t="n">
-        <v>45726.73154126157</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B525" t="inlineStr">
         <is>
@@ -19877,7 +19877,7 @@
     </row>
     <row r="526">
       <c r="A526" s="2" t="n">
-        <v>45726.73156329861</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B526" t="inlineStr">
         <is>
@@ -19914,7 +19914,7 @@
     </row>
     <row r="527">
       <c r="A527" s="2" t="n">
-        <v>45726.73156329861</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B527" t="inlineStr">
         <is>
@@ -19951,7 +19951,7 @@
     </row>
     <row r="528">
       <c r="A528" s="2" t="n">
-        <v>45726.73158645834</v>
+        <v>45726.23144357639</v>
       </c>
       <c r="B528" t="inlineStr">
         <is>
@@ -19988,38 +19988,593 @@
     </row>
     <row r="529">
       <c r="A529" s="2" t="n">
+        <v>45726.23144357639</v>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E529" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F529" t="n">
+        <v>400</v>
+      </c>
+      <c r="G529" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H529" t="n">
+        <v>400</v>
+      </c>
+      <c r="I529" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="2" t="n">
+        <v>45726.23144357639</v>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E530" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F530" t="n">
+        <v>400</v>
+      </c>
+      <c r="G530" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H530" t="n">
+        <v>400</v>
+      </c>
+      <c r="I530" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="2" t="n">
+        <v>45726.23144357639</v>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E531" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F531" t="n">
+        <v>400</v>
+      </c>
+      <c r="G531" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H531" t="n">
+        <v>400</v>
+      </c>
+      <c r="I531" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="2" t="n">
+        <v>45726.23144357639</v>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E532" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F532" t="n">
+        <v>400</v>
+      </c>
+      <c r="G532" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H532" t="n">
+        <v>400</v>
+      </c>
+      <c r="I532" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="2" t="n">
+        <v>45726.73154126157</v>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E533" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F533" t="n">
+        <v>400</v>
+      </c>
+      <c r="G533" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H533" t="n">
+        <v>400</v>
+      </c>
+      <c r="I533" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="2" t="n">
+        <v>45726.73154126157</v>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E534" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F534" t="n">
+        <v>400</v>
+      </c>
+      <c r="G534" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H534" t="n">
+        <v>400</v>
+      </c>
+      <c r="I534" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="2" t="n">
+        <v>45726.73154126157</v>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E535" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F535" t="n">
+        <v>400</v>
+      </c>
+      <c r="G535" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H535" t="n">
+        <v>400</v>
+      </c>
+      <c r="I535" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="2" t="n">
+        <v>45726.73156329861</v>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E536" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F536" t="n">
+        <v>400</v>
+      </c>
+      <c r="G536" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H536" t="n">
+        <v>400</v>
+      </c>
+      <c r="I536" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="2" t="n">
+        <v>45726.73156329861</v>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D537" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E537" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F537" t="n">
+        <v>400</v>
+      </c>
+      <c r="G537" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H537" t="n">
+        <v>400</v>
+      </c>
+      <c r="I537" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="2" t="n">
+        <v>45726.73156329861</v>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D538" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E538" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F538" t="n">
+        <v>400</v>
+      </c>
+      <c r="G538" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H538" t="n">
+        <v>400</v>
+      </c>
+      <c r="I538" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="2" t="n">
         <v>45726.73158645834</v>
       </c>
-      <c r="B529" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C529" t="inlineStr">
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D529" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E529" t="inlineStr">
+      <c r="D539" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E539" t="inlineStr">
         <is>
           <t>0xd</t>
         </is>
       </c>
-      <c r="F529" t="n">
-        <v>400</v>
-      </c>
-      <c r="G529" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H529" t="n">
-        <v>400</v>
-      </c>
-      <c r="I529" t="n">
+      <c r="F539" t="n">
+        <v>400</v>
+      </c>
+      <c r="G539" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H539" t="n">
+        <v>400</v>
+      </c>
+      <c r="I539" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="2" t="n">
+        <v>45726.73158645834</v>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D540" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E540" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F540" t="n">
+        <v>400</v>
+      </c>
+      <c r="G540" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H540" t="n">
+        <v>400</v>
+      </c>
+      <c r="I540" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="2" t="n">
+        <v>45726.73158645834</v>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D541" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E541" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F541" t="n">
+        <v>400</v>
+      </c>
+      <c r="G541" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H541" t="n">
+        <v>400</v>
+      </c>
+      <c r="I541" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="2" t="n">
+        <v>45727.23168409722</v>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D542" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E542" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F542" t="n">
+        <v>400</v>
+      </c>
+      <c r="G542" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H542" t="n">
+        <v>400</v>
+      </c>
+      <c r="I542" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="2" t="n">
+        <v>45727.23170618056</v>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E543" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F543" t="n">
+        <v>400</v>
+      </c>
+      <c r="G543" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H543" t="n">
+        <v>400</v>
+      </c>
+      <c r="I543" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="2" t="n">
+        <v>45727.23172934028</v>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E544" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F544" t="n">
+        <v>400</v>
+      </c>
+      <c r="G544" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H544" t="n">
+        <v>400</v>
+      </c>
+      <c r="I544" t="n">
         <v>13</v>
       </c>
     </row>
@@ -20034,7 +20589,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I543"/>
+  <dimension ref="A1:I558"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38221,7 +38776,7 @@
     </row>
     <row r="492">
       <c r="A492" s="2" t="n">
-        <v>45725.07911518519</v>
+        <v>45725.07909302083</v>
       </c>
       <c r="B492" t="inlineStr">
         <is>
@@ -38517,7 +39072,7 @@
     </row>
     <row r="500">
       <c r="A500" s="2" t="n">
-        <v>45725.07913833333</v>
+        <v>45725.07911518519</v>
       </c>
       <c r="B500" t="inlineStr">
         <is>
@@ -38554,7 +39109,7 @@
     </row>
     <row r="501">
       <c r="A501" s="2" t="n">
-        <v>45725.07913833333</v>
+        <v>45725.07911518519</v>
       </c>
       <c r="B501" t="inlineStr">
         <is>
@@ -38813,7 +39368,7 @@
     </row>
     <row r="508">
       <c r="A508" s="2" t="n">
-        <v>45725.57923533564</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B508" t="inlineStr">
         <is>
@@ -38850,7 +39405,7 @@
     </row>
     <row r="509">
       <c r="A509" s="2" t="n">
-        <v>45725.57923533564</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B509" t="inlineStr">
         <is>
@@ -38887,7 +39442,7 @@
     </row>
     <row r="510">
       <c r="A510" s="2" t="n">
-        <v>45725.57923533564</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B510" t="inlineStr">
         <is>
@@ -39035,7 +39590,7 @@
     </row>
     <row r="514">
       <c r="A514" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B514" t="inlineStr">
         <is>
@@ -39072,7 +39627,7 @@
     </row>
     <row r="515">
       <c r="A515" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B515" t="inlineStr">
         <is>
@@ -39109,7 +39664,7 @@
     </row>
     <row r="516">
       <c r="A516" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B516" t="inlineStr">
         <is>
@@ -39146,7 +39701,7 @@
     </row>
     <row r="517">
       <c r="A517" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B517" t="inlineStr">
         <is>
@@ -39257,7 +39812,7 @@
     </row>
     <row r="520">
       <c r="A520" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B520" t="inlineStr">
         <is>
@@ -39294,7 +39849,7 @@
     </row>
     <row r="521">
       <c r="A521" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B521" t="inlineStr">
         <is>
@@ -39331,7 +39886,7 @@
     </row>
     <row r="522">
       <c r="A522" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B522" t="inlineStr">
         <is>
@@ -39368,7 +39923,7 @@
     </row>
     <row r="523">
       <c r="A523" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B523" t="inlineStr">
         <is>
@@ -39405,7 +39960,7 @@
     </row>
     <row r="524">
       <c r="A524" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B524" t="inlineStr">
         <is>
@@ -39479,7 +40034,7 @@
     </row>
     <row r="526">
       <c r="A526" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B526" t="inlineStr">
         <is>
@@ -39516,7 +40071,7 @@
     </row>
     <row r="527">
       <c r="A527" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B527" t="inlineStr">
         <is>
@@ -39553,7 +40108,7 @@
     </row>
     <row r="528">
       <c r="A528" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B528" t="inlineStr">
         <is>
@@ -39590,7 +40145,7 @@
     </row>
     <row r="529">
       <c r="A529" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B529" t="inlineStr">
         <is>
@@ -39627,7 +40182,7 @@
     </row>
     <row r="530">
       <c r="A530" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B530" t="inlineStr">
         <is>
@@ -39664,7 +40219,7 @@
     </row>
     <row r="531">
       <c r="A531" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B531" t="inlineStr">
         <is>
@@ -39701,7 +40256,7 @@
     </row>
     <row r="532">
       <c r="A532" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B532" t="inlineStr">
         <is>
@@ -39738,7 +40293,7 @@
     </row>
     <row r="533">
       <c r="A533" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B533" t="inlineStr">
         <is>
@@ -39775,7 +40330,7 @@
     </row>
     <row r="534">
       <c r="A534" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B534" t="inlineStr">
         <is>
@@ -39812,7 +40367,7 @@
     </row>
     <row r="535">
       <c r="A535" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B535" t="inlineStr">
         <is>
@@ -39849,7 +40404,7 @@
     </row>
     <row r="536">
       <c r="A536" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B536" t="inlineStr">
         <is>
@@ -39886,7 +40441,7 @@
     </row>
     <row r="537">
       <c r="A537" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B537" t="inlineStr">
         <is>
@@ -39923,7 +40478,7 @@
     </row>
     <row r="538">
       <c r="A538" s="2" t="n">
-        <v>45726.57952</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B538" t="inlineStr">
         <is>
@@ -39960,7 +40515,7 @@
     </row>
     <row r="539">
       <c r="A539" s="2" t="n">
-        <v>45726.57952</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B539" t="inlineStr">
         <is>
@@ -39997,7 +40552,7 @@
     </row>
     <row r="540">
       <c r="A540" s="2" t="n">
-        <v>45726.57954204861</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B540" t="inlineStr">
         <is>
@@ -40034,7 +40589,7 @@
     </row>
     <row r="541">
       <c r="A541" s="2" t="n">
-        <v>45726.57954204861</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B541" t="inlineStr">
         <is>
@@ -40071,7 +40626,7 @@
     </row>
     <row r="542">
       <c r="A542" s="2" t="n">
-        <v>45726.57956549768</v>
+        <v>45726.07942256945</v>
       </c>
       <c r="B542" t="inlineStr">
         <is>
@@ -40108,38 +40663,593 @@
     </row>
     <row r="543">
       <c r="A543" s="2" t="n">
+        <v>45726.07942256945</v>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E543" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F543" t="n">
+        <v>400</v>
+      </c>
+      <c r="G543" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H543" t="n">
+        <v>400</v>
+      </c>
+      <c r="I543" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="2" t="n">
+        <v>45726.07942256945</v>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E544" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F544" t="n">
+        <v>400</v>
+      </c>
+      <c r="G544" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H544" t="n">
+        <v>400</v>
+      </c>
+      <c r="I544" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="2" t="n">
+        <v>45726.07942256945</v>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E545" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F545" t="n">
+        <v>400</v>
+      </c>
+      <c r="G545" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H545" t="n">
+        <v>400</v>
+      </c>
+      <c r="I545" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="2" t="n">
+        <v>45726.07942256945</v>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E546" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F546" t="n">
+        <v>400</v>
+      </c>
+      <c r="G546" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H546" t="n">
+        <v>400</v>
+      </c>
+      <c r="I546" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="2" t="n">
+        <v>45726.57952</v>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E547" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F547" t="n">
+        <v>400</v>
+      </c>
+      <c r="G547" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H547" t="n">
+        <v>400</v>
+      </c>
+      <c r="I547" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="2" t="n">
+        <v>45726.57952</v>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F548" t="n">
+        <v>400</v>
+      </c>
+      <c r="G548" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H548" t="n">
+        <v>400</v>
+      </c>
+      <c r="I548" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="2" t="n">
+        <v>45726.57952</v>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F549" t="n">
+        <v>400</v>
+      </c>
+      <c r="G549" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H549" t="n">
+        <v>400</v>
+      </c>
+      <c r="I549" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="2" t="n">
+        <v>45726.57954204861</v>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E550" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F550" t="n">
+        <v>400</v>
+      </c>
+      <c r="G550" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H550" t="n">
+        <v>400</v>
+      </c>
+      <c r="I550" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="2" t="n">
+        <v>45726.57954204861</v>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E551" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F551" t="n">
+        <v>400</v>
+      </c>
+      <c r="G551" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H551" t="n">
+        <v>400</v>
+      </c>
+      <c r="I551" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="2" t="n">
+        <v>45726.57954204861</v>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E552" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F552" t="n">
+        <v>400</v>
+      </c>
+      <c r="G552" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H552" t="n">
+        <v>400</v>
+      </c>
+      <c r="I552" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="2" t="n">
         <v>45726.57956549768</v>
       </c>
-      <c r="B543" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C543" t="inlineStr">
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D543" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E543" t="inlineStr">
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E553" t="inlineStr">
         <is>
           <t>0xe</t>
         </is>
       </c>
-      <c r="F543" t="n">
-        <v>400</v>
-      </c>
-      <c r="G543" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H543" t="n">
-        <v>400</v>
-      </c>
-      <c r="I543" t="n">
+      <c r="F553" t="n">
+        <v>400</v>
+      </c>
+      <c r="G553" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H553" t="n">
+        <v>400</v>
+      </c>
+      <c r="I553" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="2" t="n">
+        <v>45726.57956549768</v>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E554" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F554" t="n">
+        <v>400</v>
+      </c>
+      <c r="G554" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H554" t="n">
+        <v>400</v>
+      </c>
+      <c r="I554" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="2" t="n">
+        <v>45726.57956549768</v>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E555" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F555" t="n">
+        <v>400</v>
+      </c>
+      <c r="G555" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H555" t="n">
+        <v>400</v>
+      </c>
+      <c r="I555" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="2" t="n">
+        <v>45727.07966211806</v>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F556" t="n">
+        <v>400</v>
+      </c>
+      <c r="G556" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H556" t="n">
+        <v>400</v>
+      </c>
+      <c r="I556" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="2" t="n">
+        <v>45727.07968420139</v>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E557" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F557" t="n">
+        <v>400</v>
+      </c>
+      <c r="G557" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H557" t="n">
+        <v>400</v>
+      </c>
+      <c r="I557" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="2" t="n">
+        <v>45727.07970724537</v>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E558" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F558" t="n">
+        <v>400</v>
+      </c>
+      <c r="G558" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H558" t="n">
+        <v>400</v>
+      </c>
+      <c r="I558" t="n">
         <v>14</v>
       </c>
     </row>
@@ -56204,7 +57314,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I547"/>
+  <dimension ref="A1:I562"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -74539,7 +75649,7 @@
     </row>
     <row r="496">
       <c r="A496" s="2" t="n">
-        <v>45725.22922125</v>
+        <v>45725.22919952546</v>
       </c>
       <c r="B496" t="inlineStr">
         <is>
@@ -74835,7 +75945,7 @@
     </row>
     <row r="504">
       <c r="A504" s="2" t="n">
-        <v>45725.22924497685</v>
+        <v>45725.22922125</v>
       </c>
       <c r="B504" t="inlineStr">
         <is>
@@ -74872,7 +75982,7 @@
     </row>
     <row r="505">
       <c r="A505" s="2" t="n">
-        <v>45725.22924497685</v>
+        <v>45725.22922125</v>
       </c>
       <c r="B505" t="inlineStr">
         <is>
@@ -75131,7 +76241,7 @@
     </row>
     <row r="512">
       <c r="A512" s="2" t="n">
-        <v>45725.7293421412</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B512" t="inlineStr">
         <is>
@@ -75168,7 +76278,7 @@
     </row>
     <row r="513">
       <c r="A513" s="2" t="n">
-        <v>45725.7293421412</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B513" t="inlineStr">
         <is>
@@ -75205,7 +76315,7 @@
     </row>
     <row r="514">
       <c r="A514" s="2" t="n">
-        <v>45725.7293421412</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B514" t="inlineStr">
         <is>
@@ -75353,7 +76463,7 @@
     </row>
     <row r="518">
       <c r="A518" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B518" t="inlineStr">
         <is>
@@ -75390,7 +76500,7 @@
     </row>
     <row r="519">
       <c r="A519" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B519" t="inlineStr">
         <is>
@@ -75427,7 +76537,7 @@
     </row>
     <row r="520">
       <c r="A520" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B520" t="inlineStr">
         <is>
@@ -75464,7 +76574,7 @@
     </row>
     <row r="521">
       <c r="A521" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B521" t="inlineStr">
         <is>
@@ -75575,7 +76685,7 @@
     </row>
     <row r="524">
       <c r="A524" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B524" t="inlineStr">
         <is>
@@ -75612,7 +76722,7 @@
     </row>
     <row r="525">
       <c r="A525" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B525" t="inlineStr">
         <is>
@@ -75649,7 +76759,7 @@
     </row>
     <row r="526">
       <c r="A526" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B526" t="inlineStr">
         <is>
@@ -75686,7 +76796,7 @@
     </row>
     <row r="527">
       <c r="A527" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B527" t="inlineStr">
         <is>
@@ -75723,7 +76833,7 @@
     </row>
     <row r="528">
       <c r="A528" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B528" t="inlineStr">
         <is>
@@ -75797,7 +76907,7 @@
     </row>
     <row r="530">
       <c r="A530" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B530" t="inlineStr">
         <is>
@@ -75834,7 +76944,7 @@
     </row>
     <row r="531">
       <c r="A531" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B531" t="inlineStr">
         <is>
@@ -75871,7 +76981,7 @@
     </row>
     <row r="532">
       <c r="A532" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B532" t="inlineStr">
         <is>
@@ -75908,7 +77018,7 @@
     </row>
     <row r="533">
       <c r="A533" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B533" t="inlineStr">
         <is>
@@ -75945,7 +77055,7 @@
     </row>
     <row r="534">
       <c r="A534" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B534" t="inlineStr">
         <is>
@@ -75982,7 +77092,7 @@
     </row>
     <row r="535">
       <c r="A535" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B535" t="inlineStr">
         <is>
@@ -76019,7 +77129,7 @@
     </row>
     <row r="536">
       <c r="A536" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B536" t="inlineStr">
         <is>
@@ -76056,7 +77166,7 @@
     </row>
     <row r="537">
       <c r="A537" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B537" t="inlineStr">
         <is>
@@ -76093,7 +77203,7 @@
     </row>
     <row r="538">
       <c r="A538" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B538" t="inlineStr">
         <is>
@@ -76130,7 +77240,7 @@
     </row>
     <row r="539">
       <c r="A539" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B539" t="inlineStr">
         <is>
@@ -76167,7 +77277,7 @@
     </row>
     <row r="540">
       <c r="A540" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B540" t="inlineStr">
         <is>
@@ -76204,7 +77314,7 @@
     </row>
     <row r="541">
       <c r="A541" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B541" t="inlineStr">
         <is>
@@ -76241,7 +77351,7 @@
     </row>
     <row r="542">
       <c r="A542" s="2" t="n">
-        <v>45726.72962616898</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B542" t="inlineStr">
         <is>
@@ -76278,7 +77388,7 @@
     </row>
     <row r="543">
       <c r="A543" s="2" t="n">
-        <v>45726.72962616898</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B543" t="inlineStr">
         <is>
@@ -76315,7 +77425,7 @@
     </row>
     <row r="544">
       <c r="A544" s="2" t="n">
-        <v>45726.72964848379</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B544" t="inlineStr">
         <is>
@@ -76352,7 +77462,7 @@
     </row>
     <row r="545">
       <c r="A545" s="2" t="n">
-        <v>45726.72964848379</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B545" t="inlineStr">
         <is>
@@ -76389,7 +77499,7 @@
     </row>
     <row r="546">
       <c r="A546" s="2" t="n">
-        <v>45726.72967174769</v>
+        <v>45726.22953034722</v>
       </c>
       <c r="B546" t="inlineStr">
         <is>
@@ -76426,38 +77536,593 @@
     </row>
     <row r="547">
       <c r="A547" s="2" t="n">
+        <v>45726.22953034722</v>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E547" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F547" t="n">
+        <v>400</v>
+      </c>
+      <c r="G547" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H547" t="n">
+        <v>400</v>
+      </c>
+      <c r="I547" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="2" t="n">
+        <v>45726.22953034722</v>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F548" t="n">
+        <v>400</v>
+      </c>
+      <c r="G548" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H548" t="n">
+        <v>400</v>
+      </c>
+      <c r="I548" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="2" t="n">
+        <v>45726.22953034722</v>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F549" t="n">
+        <v>400</v>
+      </c>
+      <c r="G549" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H549" t="n">
+        <v>400</v>
+      </c>
+      <c r="I549" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="2" t="n">
+        <v>45726.22953034722</v>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E550" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F550" t="n">
+        <v>400</v>
+      </c>
+      <c r="G550" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H550" t="n">
+        <v>400</v>
+      </c>
+      <c r="I550" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="2" t="n">
+        <v>45726.72962616898</v>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E551" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F551" t="n">
+        <v>400</v>
+      </c>
+      <c r="G551" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H551" t="n">
+        <v>400</v>
+      </c>
+      <c r="I551" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="2" t="n">
+        <v>45726.72962616898</v>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E552" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F552" t="n">
+        <v>400</v>
+      </c>
+      <c r="G552" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H552" t="n">
+        <v>400</v>
+      </c>
+      <c r="I552" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="2" t="n">
+        <v>45726.72962616898</v>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E553" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F553" t="n">
+        <v>400</v>
+      </c>
+      <c r="G553" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H553" t="n">
+        <v>400</v>
+      </c>
+      <c r="I553" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="2" t="n">
+        <v>45726.72964848379</v>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E554" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F554" t="n">
+        <v>400</v>
+      </c>
+      <c r="G554" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H554" t="n">
+        <v>400</v>
+      </c>
+      <c r="I554" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="2" t="n">
+        <v>45726.72964848379</v>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E555" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F555" t="n">
+        <v>400</v>
+      </c>
+      <c r="G555" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H555" t="n">
+        <v>400</v>
+      </c>
+      <c r="I555" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="2" t="n">
+        <v>45726.72964848379</v>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F556" t="n">
+        <v>400</v>
+      </c>
+      <c r="G556" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H556" t="n">
+        <v>400</v>
+      </c>
+      <c r="I556" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="2" t="n">
         <v>45726.72967174769</v>
       </c>
-      <c r="B547" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C547" t="inlineStr">
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
         </is>
       </c>
-      <c r="D547" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E547" t="inlineStr">
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E557" t="inlineStr">
         <is>
           <t>0x3</t>
         </is>
       </c>
-      <c r="F547" t="n">
-        <v>400</v>
-      </c>
-      <c r="G547" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H547" t="n">
-        <v>400</v>
-      </c>
-      <c r="I547" t="n">
+      <c r="F557" t="n">
+        <v>400</v>
+      </c>
+      <c r="G557" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H557" t="n">
+        <v>400</v>
+      </c>
+      <c r="I557" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="2" t="n">
+        <v>45726.72967174769</v>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E558" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F558" t="n">
+        <v>400</v>
+      </c>
+      <c r="G558" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H558" t="n">
+        <v>400</v>
+      </c>
+      <c r="I558" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="2" t="n">
+        <v>45726.72967174769</v>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E559" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F559" t="n">
+        <v>400</v>
+      </c>
+      <c r="G559" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H559" t="n">
+        <v>400</v>
+      </c>
+      <c r="I559" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="2" t="n">
+        <v>45727.22976834491</v>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E560" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F560" t="n">
+        <v>400</v>
+      </c>
+      <c r="G560" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H560" t="n">
+        <v>400</v>
+      </c>
+      <c r="I560" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="2" t="n">
+        <v>45727.22979072916</v>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E561" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F561" t="n">
+        <v>400</v>
+      </c>
+      <c r="G561" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H561" t="n">
+        <v>400</v>
+      </c>
+      <c r="I561" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="2" t="n">
+        <v>45727.22981358796</v>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E562" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F562" t="n">
+        <v>400</v>
+      </c>
+      <c r="G562" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H562" t="n">
+        <v>400</v>
+      </c>
+      <c r="I562" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove image processing memory leaks
</commit_message>
<xml_diff>
--- a/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
+++ b/sensorCSV/SAG1_sensor_data_with_decimal_filtered.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I544"/>
+  <dimension ref="A1:I559"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18138,7 +18138,7 @@
     </row>
     <row r="479">
       <c r="A479" s="2" t="n">
-        <v>45725.23113506944</v>
+        <v>45725.23111297454</v>
       </c>
       <c r="B479" t="inlineStr">
         <is>
@@ -18471,7 +18471,7 @@
     </row>
     <row r="488">
       <c r="A488" s="2" t="n">
-        <v>45725.23115855324</v>
+        <v>45725.23113506944</v>
       </c>
       <c r="B488" t="inlineStr">
         <is>
@@ -18508,7 +18508,7 @@
     </row>
     <row r="489">
       <c r="A489" s="2" t="n">
-        <v>45725.23115855324</v>
+        <v>45725.23113506944</v>
       </c>
       <c r="B489" t="inlineStr">
         <is>
@@ -18804,7 +18804,7 @@
     </row>
     <row r="497">
       <c r="A497" s="2" t="n">
-        <v>45725.73125641204</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B497" t="inlineStr">
         <is>
@@ -18841,7 +18841,7 @@
     </row>
     <row r="498">
       <c r="A498" s="2" t="n">
-        <v>45725.73125641204</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B498" t="inlineStr">
         <is>
@@ -18878,7 +18878,7 @@
     </row>
     <row r="499">
       <c r="A499" s="2" t="n">
-        <v>45725.73125641204</v>
+        <v>45725.23115855324</v>
       </c>
       <c r="B499" t="inlineStr">
         <is>
@@ -19063,7 +19063,7 @@
     </row>
     <row r="504">
       <c r="A504" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B504" t="inlineStr">
         <is>
@@ -19100,7 +19100,7 @@
     </row>
     <row r="505">
       <c r="A505" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B505" t="inlineStr">
         <is>
@@ -19137,7 +19137,7 @@
     </row>
     <row r="506">
       <c r="A506" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B506" t="inlineStr">
         <is>
@@ -19174,7 +19174,7 @@
     </row>
     <row r="507">
       <c r="A507" s="2" t="n">
-        <v>45725.73127832176</v>
+        <v>45725.73125641204</v>
       </c>
       <c r="B507" t="inlineStr">
         <is>
@@ -19322,7 +19322,7 @@
     </row>
     <row r="511">
       <c r="A511" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B511" t="inlineStr">
         <is>
@@ -19359,7 +19359,7 @@
     </row>
     <row r="512">
       <c r="A512" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B512" t="inlineStr">
         <is>
@@ -19396,7 +19396,7 @@
     </row>
     <row r="513">
       <c r="A513" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B513" t="inlineStr">
         <is>
@@ -19433,7 +19433,7 @@
     </row>
     <row r="514">
       <c r="A514" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B514" t="inlineStr">
         <is>
@@ -19470,7 +19470,7 @@
     </row>
     <row r="515">
       <c r="A515" s="2" t="n">
-        <v>45725.73130123843</v>
+        <v>45725.73127832176</v>
       </c>
       <c r="B515" t="inlineStr">
         <is>
@@ -19581,7 +19581,7 @@
     </row>
     <row r="518">
       <c r="A518" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B518" t="inlineStr">
         <is>
@@ -19618,7 +19618,7 @@
     </row>
     <row r="519">
       <c r="A519" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B519" t="inlineStr">
         <is>
@@ -19655,7 +19655,7 @@
     </row>
     <row r="520">
       <c r="A520" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B520" t="inlineStr">
         <is>
@@ -19692,7 +19692,7 @@
     </row>
     <row r="521">
       <c r="A521" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B521" t="inlineStr">
         <is>
@@ -19729,7 +19729,7 @@
     </row>
     <row r="522">
       <c r="A522" s="2" t="n">
-        <v>45726.23139893518</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B522" t="inlineStr">
         <is>
@@ -19766,7 +19766,7 @@
     </row>
     <row r="523">
       <c r="A523" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45725.73130123843</v>
       </c>
       <c r="B523" t="inlineStr">
         <is>
@@ -19803,7 +19803,7 @@
     </row>
     <row r="524">
       <c r="A524" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B524" t="inlineStr">
         <is>
@@ -19840,7 +19840,7 @@
     </row>
     <row r="525">
       <c r="A525" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B525" t="inlineStr">
         <is>
@@ -19877,7 +19877,7 @@
     </row>
     <row r="526">
       <c r="A526" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B526" t="inlineStr">
         <is>
@@ -19914,7 +19914,7 @@
     </row>
     <row r="527">
       <c r="A527" s="2" t="n">
-        <v>45726.23142038195</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B527" t="inlineStr">
         <is>
@@ -19951,7 +19951,7 @@
     </row>
     <row r="528">
       <c r="A528" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B528" t="inlineStr">
         <is>
@@ -19988,7 +19988,7 @@
     </row>
     <row r="529">
       <c r="A529" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23139893518</v>
       </c>
       <c r="B529" t="inlineStr">
         <is>
@@ -20025,7 +20025,7 @@
     </row>
     <row r="530">
       <c r="A530" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B530" t="inlineStr">
         <is>
@@ -20062,7 +20062,7 @@
     </row>
     <row r="531">
       <c r="A531" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B531" t="inlineStr">
         <is>
@@ -20099,7 +20099,7 @@
     </row>
     <row r="532">
       <c r="A532" s="2" t="n">
-        <v>45726.23144357639</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B532" t="inlineStr">
         <is>
@@ -20136,7 +20136,7 @@
     </row>
     <row r="533">
       <c r="A533" s="2" t="n">
-        <v>45726.73154126157</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B533" t="inlineStr">
         <is>
@@ -20173,7 +20173,7 @@
     </row>
     <row r="534">
       <c r="A534" s="2" t="n">
-        <v>45726.73154126157</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B534" t="inlineStr">
         <is>
@@ -20210,7 +20210,7 @@
     </row>
     <row r="535">
       <c r="A535" s="2" t="n">
-        <v>45726.73154126157</v>
+        <v>45726.23142038195</v>
       </c>
       <c r="B535" t="inlineStr">
         <is>
@@ -20247,7 +20247,7 @@
     </row>
     <row r="536">
       <c r="A536" s="2" t="n">
-        <v>45726.73156329861</v>
+        <v>45726.23144357639</v>
       </c>
       <c r="B536" t="inlineStr">
         <is>
@@ -20284,7 +20284,7 @@
     </row>
     <row r="537">
       <c r="A537" s="2" t="n">
-        <v>45726.73156329861</v>
+        <v>45726.23144357639</v>
       </c>
       <c r="B537" t="inlineStr">
         <is>
@@ -20321,7 +20321,7 @@
     </row>
     <row r="538">
       <c r="A538" s="2" t="n">
-        <v>45726.73156329861</v>
+        <v>45726.23144357639</v>
       </c>
       <c r="B538" t="inlineStr">
         <is>
@@ -20358,7 +20358,7 @@
     </row>
     <row r="539">
       <c r="A539" s="2" t="n">
-        <v>45726.73158645834</v>
+        <v>45726.23144357639</v>
       </c>
       <c r="B539" t="inlineStr">
         <is>
@@ -20395,7 +20395,7 @@
     </row>
     <row r="540">
       <c r="A540" s="2" t="n">
-        <v>45726.73158645834</v>
+        <v>45726.23144357639</v>
       </c>
       <c r="B540" t="inlineStr">
         <is>
@@ -20432,7 +20432,7 @@
     </row>
     <row r="541">
       <c r="A541" s="2" t="n">
-        <v>45726.73158645834</v>
+        <v>45726.23144357639</v>
       </c>
       <c r="B541" t="inlineStr">
         <is>
@@ -20469,7 +20469,7 @@
     </row>
     <row r="542">
       <c r="A542" s="2" t="n">
-        <v>45727.23168409722</v>
+        <v>45726.73154126157</v>
       </c>
       <c r="B542" t="inlineStr">
         <is>
@@ -20506,7 +20506,7 @@
     </row>
     <row r="543">
       <c r="A543" s="2" t="n">
-        <v>45727.23170618056</v>
+        <v>45726.73154126157</v>
       </c>
       <c r="B543" t="inlineStr">
         <is>
@@ -20543,38 +20543,593 @@
     </row>
     <row r="544">
       <c r="A544" s="2" t="n">
+        <v>45726.73154126157</v>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E544" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F544" t="n">
+        <v>400</v>
+      </c>
+      <c r="G544" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H544" t="n">
+        <v>400</v>
+      </c>
+      <c r="I544" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="2" t="n">
+        <v>45726.73154126157</v>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E545" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F545" t="n">
+        <v>400</v>
+      </c>
+      <c r="G545" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H545" t="n">
+        <v>400</v>
+      </c>
+      <c r="I545" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="2" t="n">
+        <v>45726.73156329861</v>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E546" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F546" t="n">
+        <v>400</v>
+      </c>
+      <c r="G546" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H546" t="n">
+        <v>400</v>
+      </c>
+      <c r="I546" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="2" t="n">
+        <v>45726.73156329861</v>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E547" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F547" t="n">
+        <v>400</v>
+      </c>
+      <c r="G547" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H547" t="n">
+        <v>400</v>
+      </c>
+      <c r="I547" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="2" t="n">
+        <v>45726.73156329861</v>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F548" t="n">
+        <v>400</v>
+      </c>
+      <c r="G548" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H548" t="n">
+        <v>400</v>
+      </c>
+      <c r="I548" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="2" t="n">
+        <v>45726.73156329861</v>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F549" t="n">
+        <v>400</v>
+      </c>
+      <c r="G549" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H549" t="n">
+        <v>400</v>
+      </c>
+      <c r="I549" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="2" t="n">
+        <v>45726.73158645834</v>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E550" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F550" t="n">
+        <v>400</v>
+      </c>
+      <c r="G550" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H550" t="n">
+        <v>400</v>
+      </c>
+      <c r="I550" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="2" t="n">
+        <v>45726.73158645834</v>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E551" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F551" t="n">
+        <v>400</v>
+      </c>
+      <c r="G551" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H551" t="n">
+        <v>400</v>
+      </c>
+      <c r="I551" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="2" t="n">
+        <v>45726.73158645834</v>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E552" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F552" t="n">
+        <v>400</v>
+      </c>
+      <c r="G552" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H552" t="n">
+        <v>400</v>
+      </c>
+      <c r="I552" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="2" t="n">
+        <v>45726.73158645834</v>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E553" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F553" t="n">
+        <v>400</v>
+      </c>
+      <c r="G553" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H553" t="n">
+        <v>400</v>
+      </c>
+      <c r="I553" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="2" t="n">
+        <v>45727.23168409722</v>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E554" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F554" t="n">
+        <v>400</v>
+      </c>
+      <c r="G554" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H554" t="n">
+        <v>400</v>
+      </c>
+      <c r="I554" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="2" t="n">
+        <v>45727.23168409722</v>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E555" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F555" t="n">
+        <v>400</v>
+      </c>
+      <c r="G555" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H555" t="n">
+        <v>400</v>
+      </c>
+      <c r="I555" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="2" t="n">
+        <v>45727.23170618056</v>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F556" t="n">
+        <v>400</v>
+      </c>
+      <c r="G556" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H556" t="n">
+        <v>400</v>
+      </c>
+      <c r="I556" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="2" t="n">
+        <v>45727.23170618056</v>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E557" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F557" t="n">
+        <v>400</v>
+      </c>
+      <c r="G557" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H557" t="n">
+        <v>400</v>
+      </c>
+      <c r="I557" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="2" t="n">
         <v>45727.23172934028</v>
       </c>
-      <c r="B544" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C544" t="inlineStr">
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D544" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E544" t="inlineStr">
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E558" t="inlineStr">
         <is>
           <t>0xd</t>
         </is>
       </c>
-      <c r="F544" t="n">
-        <v>400</v>
-      </c>
-      <c r="G544" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H544" t="n">
-        <v>400</v>
-      </c>
-      <c r="I544" t="n">
+      <c r="F558" t="n">
+        <v>400</v>
+      </c>
+      <c r="G558" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H558" t="n">
+        <v>400</v>
+      </c>
+      <c r="I558" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="2" t="n">
+        <v>45727.23172934028</v>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E559" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F559" t="n">
+        <v>400</v>
+      </c>
+      <c r="G559" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H559" t="n">
+        <v>400</v>
+      </c>
+      <c r="I559" t="n">
         <v>13</v>
       </c>
     </row>
@@ -20589,7 +21144,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I558"/>
+  <dimension ref="A1:I573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38813,7 +39368,7 @@
     </row>
     <row r="493">
       <c r="A493" s="2" t="n">
-        <v>45725.07911518519</v>
+        <v>45725.07909302083</v>
       </c>
       <c r="B493" t="inlineStr">
         <is>
@@ -39146,7 +39701,7 @@
     </row>
     <row r="502">
       <c r="A502" s="2" t="n">
-        <v>45725.07913833333</v>
+        <v>45725.07911518519</v>
       </c>
       <c r="B502" t="inlineStr">
         <is>
@@ -39183,7 +39738,7 @@
     </row>
     <row r="503">
       <c r="A503" s="2" t="n">
-        <v>45725.07913833333</v>
+        <v>45725.07911518519</v>
       </c>
       <c r="B503" t="inlineStr">
         <is>
@@ -39479,7 +40034,7 @@
     </row>
     <row r="511">
       <c r="A511" s="2" t="n">
-        <v>45725.57923533564</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B511" t="inlineStr">
         <is>
@@ -39516,7 +40071,7 @@
     </row>
     <row r="512">
       <c r="A512" s="2" t="n">
-        <v>45725.57923533564</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B512" t="inlineStr">
         <is>
@@ -39553,7 +40108,7 @@
     </row>
     <row r="513">
       <c r="A513" s="2" t="n">
-        <v>45725.57923533564</v>
+        <v>45725.07913833333</v>
       </c>
       <c r="B513" t="inlineStr">
         <is>
@@ -39738,7 +40293,7 @@
     </row>
     <row r="518">
       <c r="A518" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B518" t="inlineStr">
         <is>
@@ -39775,7 +40330,7 @@
     </row>
     <row r="519">
       <c r="A519" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B519" t="inlineStr">
         <is>
@@ -39812,7 +40367,7 @@
     </row>
     <row r="520">
       <c r="A520" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B520" t="inlineStr">
         <is>
@@ -39849,7 +40404,7 @@
     </row>
     <row r="521">
       <c r="A521" s="2" t="n">
-        <v>45725.57925716435</v>
+        <v>45725.57923533564</v>
       </c>
       <c r="B521" t="inlineStr">
         <is>
@@ -39997,7 +40552,7 @@
     </row>
     <row r="525">
       <c r="A525" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B525" t="inlineStr">
         <is>
@@ -40034,7 +40589,7 @@
     </row>
     <row r="526">
       <c r="A526" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B526" t="inlineStr">
         <is>
@@ -40071,7 +40626,7 @@
     </row>
     <row r="527">
       <c r="A527" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B527" t="inlineStr">
         <is>
@@ -40108,7 +40663,7 @@
     </row>
     <row r="528">
       <c r="A528" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B528" t="inlineStr">
         <is>
@@ -40145,7 +40700,7 @@
     </row>
     <row r="529">
       <c r="A529" s="2" t="n">
-        <v>45725.57928042824</v>
+        <v>45725.57925716435</v>
       </c>
       <c r="B529" t="inlineStr">
         <is>
@@ -40256,7 +40811,7 @@
     </row>
     <row r="532">
       <c r="A532" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B532" t="inlineStr">
         <is>
@@ -40293,7 +40848,7 @@
     </row>
     <row r="533">
       <c r="A533" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B533" t="inlineStr">
         <is>
@@ -40330,7 +40885,7 @@
     </row>
     <row r="534">
       <c r="A534" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B534" t="inlineStr">
         <is>
@@ -40367,7 +40922,7 @@
     </row>
     <row r="535">
       <c r="A535" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B535" t="inlineStr">
         <is>
@@ -40404,7 +40959,7 @@
     </row>
     <row r="536">
       <c r="A536" s="2" t="n">
-        <v>45726.07937777778</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B536" t="inlineStr">
         <is>
@@ -40441,7 +40996,7 @@
     </row>
     <row r="537">
       <c r="A537" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45725.57928042824</v>
       </c>
       <c r="B537" t="inlineStr">
         <is>
@@ -40478,7 +41033,7 @@
     </row>
     <row r="538">
       <c r="A538" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B538" t="inlineStr">
         <is>
@@ -40515,7 +41070,7 @@
     </row>
     <row r="539">
       <c r="A539" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B539" t="inlineStr">
         <is>
@@ -40552,7 +41107,7 @@
     </row>
     <row r="540">
       <c r="A540" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B540" t="inlineStr">
         <is>
@@ -40589,7 +41144,7 @@
     </row>
     <row r="541">
       <c r="A541" s="2" t="n">
-        <v>45726.07939922454</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B541" t="inlineStr">
         <is>
@@ -40626,7 +41181,7 @@
     </row>
     <row r="542">
       <c r="A542" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B542" t="inlineStr">
         <is>
@@ -40663,7 +41218,7 @@
     </row>
     <row r="543">
       <c r="A543" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07937777778</v>
       </c>
       <c r="B543" t="inlineStr">
         <is>
@@ -40700,7 +41255,7 @@
     </row>
     <row r="544">
       <c r="A544" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B544" t="inlineStr">
         <is>
@@ -40737,7 +41292,7 @@
     </row>
     <row r="545">
       <c r="A545" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B545" t="inlineStr">
         <is>
@@ -40774,7 +41329,7 @@
     </row>
     <row r="546">
       <c r="A546" s="2" t="n">
-        <v>45726.07942256945</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B546" t="inlineStr">
         <is>
@@ -40811,7 +41366,7 @@
     </row>
     <row r="547">
       <c r="A547" s="2" t="n">
-        <v>45726.57952</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B547" t="inlineStr">
         <is>
@@ -40848,7 +41403,7 @@
     </row>
     <row r="548">
       <c r="A548" s="2" t="n">
-        <v>45726.57952</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B548" t="inlineStr">
         <is>
@@ -40885,7 +41440,7 @@
     </row>
     <row r="549">
       <c r="A549" s="2" t="n">
-        <v>45726.57952</v>
+        <v>45726.07939922454</v>
       </c>
       <c r="B549" t="inlineStr">
         <is>
@@ -40922,7 +41477,7 @@
     </row>
     <row r="550">
       <c r="A550" s="2" t="n">
-        <v>45726.57954204861</v>
+        <v>45726.07942256945</v>
       </c>
       <c r="B550" t="inlineStr">
         <is>
@@ -40959,7 +41514,7 @@
     </row>
     <row r="551">
       <c r="A551" s="2" t="n">
-        <v>45726.57954204861</v>
+        <v>45726.07942256945</v>
       </c>
       <c r="B551" t="inlineStr">
         <is>
@@ -40996,7 +41551,7 @@
     </row>
     <row r="552">
       <c r="A552" s="2" t="n">
-        <v>45726.57954204861</v>
+        <v>45726.07942256945</v>
       </c>
       <c r="B552" t="inlineStr">
         <is>
@@ -41033,7 +41588,7 @@
     </row>
     <row r="553">
       <c r="A553" s="2" t="n">
-        <v>45726.57956549768</v>
+        <v>45726.07942256945</v>
       </c>
       <c r="B553" t="inlineStr">
         <is>
@@ -41070,7 +41625,7 @@
     </row>
     <row r="554">
       <c r="A554" s="2" t="n">
-        <v>45726.57956549768</v>
+        <v>45726.07942256945</v>
       </c>
       <c r="B554" t="inlineStr">
         <is>
@@ -41107,7 +41662,7 @@
     </row>
     <row r="555">
       <c r="A555" s="2" t="n">
-        <v>45726.57956549768</v>
+        <v>45726.07942256945</v>
       </c>
       <c r="B555" t="inlineStr">
         <is>
@@ -41144,7 +41699,7 @@
     </row>
     <row r="556">
       <c r="A556" s="2" t="n">
-        <v>45727.07966211806</v>
+        <v>45726.57952</v>
       </c>
       <c r="B556" t="inlineStr">
         <is>
@@ -41181,7 +41736,7 @@
     </row>
     <row r="557">
       <c r="A557" s="2" t="n">
-        <v>45727.07968420139</v>
+        <v>45726.57952</v>
       </c>
       <c r="B557" t="inlineStr">
         <is>
@@ -41218,38 +41773,593 @@
     </row>
     <row r="558">
       <c r="A558" s="2" t="n">
+        <v>45726.57952</v>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E558" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F558" t="n">
+        <v>400</v>
+      </c>
+      <c r="G558" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H558" t="n">
+        <v>400</v>
+      </c>
+      <c r="I558" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="2" t="n">
+        <v>45726.57952</v>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E559" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F559" t="n">
+        <v>400</v>
+      </c>
+      <c r="G559" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H559" t="n">
+        <v>400</v>
+      </c>
+      <c r="I559" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="2" t="n">
+        <v>45726.57954204861</v>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E560" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F560" t="n">
+        <v>400</v>
+      </c>
+      <c r="G560" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H560" t="n">
+        <v>400</v>
+      </c>
+      <c r="I560" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="2" t="n">
+        <v>45726.57954204861</v>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E561" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F561" t="n">
+        <v>400</v>
+      </c>
+      <c r="G561" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H561" t="n">
+        <v>400</v>
+      </c>
+      <c r="I561" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="2" t="n">
+        <v>45726.57954204861</v>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E562" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F562" t="n">
+        <v>400</v>
+      </c>
+      <c r="G562" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H562" t="n">
+        <v>400</v>
+      </c>
+      <c r="I562" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="2" t="n">
+        <v>45726.57954204861</v>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E563" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F563" t="n">
+        <v>400</v>
+      </c>
+      <c r="G563" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H563" t="n">
+        <v>400</v>
+      </c>
+      <c r="I563" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="2" t="n">
+        <v>45726.57956549768</v>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E564" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F564" t="n">
+        <v>400</v>
+      </c>
+      <c r="G564" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H564" t="n">
+        <v>400</v>
+      </c>
+      <c r="I564" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="2" t="n">
+        <v>45726.57956549768</v>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E565" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F565" t="n">
+        <v>400</v>
+      </c>
+      <c r="G565" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H565" t="n">
+        <v>400</v>
+      </c>
+      <c r="I565" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="2" t="n">
+        <v>45726.57956549768</v>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E566" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F566" t="n">
+        <v>400</v>
+      </c>
+      <c r="G566" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H566" t="n">
+        <v>400</v>
+      </c>
+      <c r="I566" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="2" t="n">
+        <v>45726.57956549768</v>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E567" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F567" t="n">
+        <v>400</v>
+      </c>
+      <c r="G567" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H567" t="n">
+        <v>400</v>
+      </c>
+      <c r="I567" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="2" t="n">
+        <v>45727.07966211806</v>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E568" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F568" t="n">
+        <v>400</v>
+      </c>
+      <c r="G568" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H568" t="n">
+        <v>400</v>
+      </c>
+      <c r="I568" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="2" t="n">
+        <v>45727.07966211806</v>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E569" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F569" t="n">
+        <v>400</v>
+      </c>
+      <c r="G569" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H569" t="n">
+        <v>400</v>
+      </c>
+      <c r="I569" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="2" t="n">
+        <v>45727.07968420139</v>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E570" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F570" t="n">
+        <v>400</v>
+      </c>
+      <c r="G570" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H570" t="n">
+        <v>400</v>
+      </c>
+      <c r="I570" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="2" t="n">
+        <v>45727.07968420139</v>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E571" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F571" t="n">
+        <v>400</v>
+      </c>
+      <c r="G571" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H571" t="n">
+        <v>400</v>
+      </c>
+      <c r="I571" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="2" t="n">
         <v>45727.07970724537</v>
       </c>
-      <c r="B558" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C558" t="inlineStr">
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
         </is>
       </c>
-      <c r="D558" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E558" t="inlineStr">
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E572" t="inlineStr">
         <is>
           <t>0xe</t>
         </is>
       </c>
-      <c r="F558" t="n">
-        <v>400</v>
-      </c>
-      <c r="G558" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H558" t="n">
-        <v>400</v>
-      </c>
-      <c r="I558" t="n">
+      <c r="F572" t="n">
+        <v>400</v>
+      </c>
+      <c r="G572" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H572" t="n">
+        <v>400</v>
+      </c>
+      <c r="I572" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="2" t="n">
+        <v>45727.07970724537</v>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E573" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F573" t="n">
+        <v>400</v>
+      </c>
+      <c r="G573" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H573" t="n">
+        <v>400</v>
+      </c>
+      <c r="I573" t="n">
         <v>14</v>
       </c>
     </row>
@@ -57314,7 +58424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I562"/>
+  <dimension ref="A1:I577"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -75686,7 +76796,7 @@
     </row>
     <row r="497">
       <c r="A497" s="2" t="n">
-        <v>45725.22922125</v>
+        <v>45725.22919952546</v>
       </c>
       <c r="B497" t="inlineStr">
         <is>
@@ -76019,7 +77129,7 @@
     </row>
     <row r="506">
       <c r="A506" s="2" t="n">
-        <v>45725.22924497685</v>
+        <v>45725.22922125</v>
       </c>
       <c r="B506" t="inlineStr">
         <is>
@@ -76056,7 +77166,7 @@
     </row>
     <row r="507">
       <c r="A507" s="2" t="n">
-        <v>45725.22924497685</v>
+        <v>45725.22922125</v>
       </c>
       <c r="B507" t="inlineStr">
         <is>
@@ -76352,7 +77462,7 @@
     </row>
     <row r="515">
       <c r="A515" s="2" t="n">
-        <v>45725.7293421412</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B515" t="inlineStr">
         <is>
@@ -76389,7 +77499,7 @@
     </row>
     <row r="516">
       <c r="A516" s="2" t="n">
-        <v>45725.7293421412</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B516" t="inlineStr">
         <is>
@@ -76426,7 +77536,7 @@
     </row>
     <row r="517">
       <c r="A517" s="2" t="n">
-        <v>45725.7293421412</v>
+        <v>45725.22924497685</v>
       </c>
       <c r="B517" t="inlineStr">
         <is>
@@ -76611,7 +77721,7 @@
     </row>
     <row r="522">
       <c r="A522" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B522" t="inlineStr">
         <is>
@@ -76648,7 +77758,7 @@
     </row>
     <row r="523">
       <c r="A523" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B523" t="inlineStr">
         <is>
@@ -76685,7 +77795,7 @@
     </row>
     <row r="524">
       <c r="A524" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B524" t="inlineStr">
         <is>
@@ -76722,7 +77832,7 @@
     </row>
     <row r="525">
       <c r="A525" s="2" t="n">
-        <v>45725.72936453704</v>
+        <v>45725.7293421412</v>
       </c>
       <c r="B525" t="inlineStr">
         <is>
@@ -76870,7 +77980,7 @@
     </row>
     <row r="529">
       <c r="A529" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B529" t="inlineStr">
         <is>
@@ -76907,7 +78017,7 @@
     </row>
     <row r="530">
       <c r="A530" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B530" t="inlineStr">
         <is>
@@ -76944,7 +78054,7 @@
     </row>
     <row r="531">
       <c r="A531" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B531" t="inlineStr">
         <is>
@@ -76981,7 +78091,7 @@
     </row>
     <row r="532">
       <c r="A532" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B532" t="inlineStr">
         <is>
@@ -77018,7 +78128,7 @@
     </row>
     <row r="533">
       <c r="A533" s="2" t="n">
-        <v>45725.7293875</v>
+        <v>45725.72936453704</v>
       </c>
       <c r="B533" t="inlineStr">
         <is>
@@ -77129,7 +78239,7 @@
     </row>
     <row r="536">
       <c r="A536" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B536" t="inlineStr">
         <is>
@@ -77166,7 +78276,7 @@
     </row>
     <row r="537">
       <c r="A537" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B537" t="inlineStr">
         <is>
@@ -77203,7 +78313,7 @@
     </row>
     <row r="538">
       <c r="A538" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B538" t="inlineStr">
         <is>
@@ -77240,7 +78350,7 @@
     </row>
     <row r="539">
       <c r="A539" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B539" t="inlineStr">
         <is>
@@ -77277,7 +78387,7 @@
     </row>
     <row r="540">
       <c r="A540" s="2" t="n">
-        <v>45726.2294844213</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B540" t="inlineStr">
         <is>
@@ -77314,7 +78424,7 @@
     </row>
     <row r="541">
       <c r="A541" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45725.7293875</v>
       </c>
       <c r="B541" t="inlineStr">
         <is>
@@ -77351,7 +78461,7 @@
     </row>
     <row r="542">
       <c r="A542" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B542" t="inlineStr">
         <is>
@@ -77388,7 +78498,7 @@
     </row>
     <row r="543">
       <c r="A543" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B543" t="inlineStr">
         <is>
@@ -77425,7 +78535,7 @@
     </row>
     <row r="544">
       <c r="A544" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B544" t="inlineStr">
         <is>
@@ -77462,7 +78572,7 @@
     </row>
     <row r="545">
       <c r="A545" s="2" t="n">
-        <v>45726.22950657408</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B545" t="inlineStr">
         <is>
@@ -77499,7 +78609,7 @@
     </row>
     <row r="546">
       <c r="A546" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B546" t="inlineStr">
         <is>
@@ -77536,7 +78646,7 @@
     </row>
     <row r="547">
       <c r="A547" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.2294844213</v>
       </c>
       <c r="B547" t="inlineStr">
         <is>
@@ -77573,7 +78683,7 @@
     </row>
     <row r="548">
       <c r="A548" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B548" t="inlineStr">
         <is>
@@ -77610,7 +78720,7 @@
     </row>
     <row r="549">
       <c r="A549" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B549" t="inlineStr">
         <is>
@@ -77647,7 +78757,7 @@
     </row>
     <row r="550">
       <c r="A550" s="2" t="n">
-        <v>45726.22953034722</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B550" t="inlineStr">
         <is>
@@ -77684,7 +78794,7 @@
     </row>
     <row r="551">
       <c r="A551" s="2" t="n">
-        <v>45726.72962616898</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B551" t="inlineStr">
         <is>
@@ -77721,7 +78831,7 @@
     </row>
     <row r="552">
       <c r="A552" s="2" t="n">
-        <v>45726.72962616898</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B552" t="inlineStr">
         <is>
@@ -77758,7 +78868,7 @@
     </row>
     <row r="553">
       <c r="A553" s="2" t="n">
-        <v>45726.72962616898</v>
+        <v>45726.22950657408</v>
       </c>
       <c r="B553" t="inlineStr">
         <is>
@@ -77795,7 +78905,7 @@
     </row>
     <row r="554">
       <c r="A554" s="2" t="n">
-        <v>45726.72964848379</v>
+        <v>45726.22953034722</v>
       </c>
       <c r="B554" t="inlineStr">
         <is>
@@ -77832,7 +78942,7 @@
     </row>
     <row r="555">
       <c r="A555" s="2" t="n">
-        <v>45726.72964848379</v>
+        <v>45726.22953034722</v>
       </c>
       <c r="B555" t="inlineStr">
         <is>
@@ -77869,7 +78979,7 @@
     </row>
     <row r="556">
       <c r="A556" s="2" t="n">
-        <v>45726.72964848379</v>
+        <v>45726.22953034722</v>
       </c>
       <c r="B556" t="inlineStr">
         <is>
@@ -77906,7 +79016,7 @@
     </row>
     <row r="557">
       <c r="A557" s="2" t="n">
-        <v>45726.72967174769</v>
+        <v>45726.22953034722</v>
       </c>
       <c r="B557" t="inlineStr">
         <is>
@@ -77943,7 +79053,7 @@
     </row>
     <row r="558">
       <c r="A558" s="2" t="n">
-        <v>45726.72967174769</v>
+        <v>45726.22953034722</v>
       </c>
       <c r="B558" t="inlineStr">
         <is>
@@ -77980,7 +79090,7 @@
     </row>
     <row r="559">
       <c r="A559" s="2" t="n">
-        <v>45726.72967174769</v>
+        <v>45726.22953034722</v>
       </c>
       <c r="B559" t="inlineStr">
         <is>
@@ -78017,7 +79127,7 @@
     </row>
     <row r="560">
       <c r="A560" s="2" t="n">
-        <v>45727.22976834491</v>
+        <v>45726.72962616898</v>
       </c>
       <c r="B560" t="inlineStr">
         <is>
@@ -78054,7 +79164,7 @@
     </row>
     <row r="561">
       <c r="A561" s="2" t="n">
-        <v>45727.22979072916</v>
+        <v>45726.72962616898</v>
       </c>
       <c r="B561" t="inlineStr">
         <is>
@@ -78091,38 +79201,593 @@
     </row>
     <row r="562">
       <c r="A562" s="2" t="n">
+        <v>45726.72962616898</v>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E562" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F562" t="n">
+        <v>400</v>
+      </c>
+      <c r="G562" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H562" t="n">
+        <v>400</v>
+      </c>
+      <c r="I562" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="2" t="n">
+        <v>45726.72962616898</v>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E563" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F563" t="n">
+        <v>400</v>
+      </c>
+      <c r="G563" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H563" t="n">
+        <v>400</v>
+      </c>
+      <c r="I563" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="2" t="n">
+        <v>45726.72964848379</v>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E564" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F564" t="n">
+        <v>400</v>
+      </c>
+      <c r="G564" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H564" t="n">
+        <v>400</v>
+      </c>
+      <c r="I564" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="2" t="n">
+        <v>45726.72964848379</v>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E565" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F565" t="n">
+        <v>400</v>
+      </c>
+      <c r="G565" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H565" t="n">
+        <v>400</v>
+      </c>
+      <c r="I565" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="2" t="n">
+        <v>45726.72964848379</v>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E566" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F566" t="n">
+        <v>400</v>
+      </c>
+      <c r="G566" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H566" t="n">
+        <v>400</v>
+      </c>
+      <c r="I566" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="2" t="n">
+        <v>45726.72964848379</v>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E567" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F567" t="n">
+        <v>400</v>
+      </c>
+      <c r="G567" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H567" t="n">
+        <v>400</v>
+      </c>
+      <c r="I567" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="2" t="n">
+        <v>45726.72967174769</v>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E568" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F568" t="n">
+        <v>400</v>
+      </c>
+      <c r="G568" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H568" t="n">
+        <v>400</v>
+      </c>
+      <c r="I568" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="2" t="n">
+        <v>45726.72967174769</v>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E569" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F569" t="n">
+        <v>400</v>
+      </c>
+      <c r="G569" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H569" t="n">
+        <v>400</v>
+      </c>
+      <c r="I569" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="2" t="n">
+        <v>45726.72967174769</v>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E570" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F570" t="n">
+        <v>400</v>
+      </c>
+      <c r="G570" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H570" t="n">
+        <v>400</v>
+      </c>
+      <c r="I570" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="2" t="n">
+        <v>45726.72967174769</v>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E571" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F571" t="n">
+        <v>400</v>
+      </c>
+      <c r="G571" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H571" t="n">
+        <v>400</v>
+      </c>
+      <c r="I571" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="2" t="n">
+        <v>45727.22976834491</v>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E572" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F572" t="n">
+        <v>400</v>
+      </c>
+      <c r="G572" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H572" t="n">
+        <v>400</v>
+      </c>
+      <c r="I572" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="2" t="n">
+        <v>45727.22976834491</v>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E573" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F573" t="n">
+        <v>400</v>
+      </c>
+      <c r="G573" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H573" t="n">
+        <v>400</v>
+      </c>
+      <c r="I573" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="2" t="n">
+        <v>45727.22979072916</v>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E574" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F574" t="n">
+        <v>400</v>
+      </c>
+      <c r="G574" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H574" t="n">
+        <v>400</v>
+      </c>
+      <c r="I574" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="2" t="n">
+        <v>45727.22979072916</v>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E575" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F575" t="n">
+        <v>400</v>
+      </c>
+      <c r="G575" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H575" t="n">
+        <v>400</v>
+      </c>
+      <c r="I575" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="2" t="n">
         <v>45727.22981358796</v>
       </c>
-      <c r="B562" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C562" t="inlineStr">
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
         <is>
           <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
         </is>
       </c>
-      <c r="D562" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E562" t="inlineStr">
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr">
         <is>
           <t>0x3</t>
         </is>
       </c>
-      <c r="F562" t="n">
-        <v>400</v>
-      </c>
-      <c r="G562" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H562" t="n">
-        <v>400</v>
-      </c>
-      <c r="I562" t="n">
+      <c r="F576" t="n">
+        <v>400</v>
+      </c>
+      <c r="G576" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H576" t="n">
+        <v>400</v>
+      </c>
+      <c r="I576" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="2" t="n">
+        <v>45727.22981358796</v>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E577" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F577" t="n">
+        <v>400</v>
+      </c>
+      <c r="G577" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H577" t="n">
+        <v>400</v>
+      </c>
+      <c r="I577" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>